<commit_message>
Added presentation dir and update Zeitplan
Manuel
</commit_message>
<xml_diff>
--- a/Zeitplan/Aktueller Zeitplan.xlsx
+++ b/Zeitplan/Aktueller Zeitplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Info\Projects\Uniprojekt\Zeitplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Info\Projects\UniprojektGitHub\Zeitplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A2D83F-E665-43D0-BD8B-438B1C0D8F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFDF292-76D3-498C-A2FE-05988195E08B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{3BCD9E55-44D3-4FC7-AA79-02F85DDF559B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="40">
   <si>
     <t xml:space="preserve">Tag </t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -773,6 +773,9 @@
       <c r="J5" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K5" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -805,7 +808,9 @@
       <c r="J6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -838,6 +843,9 @@
       <c r="J7" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K7" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -870,6 +878,9 @@
       <c r="J8" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K8" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -900,6 +911,9 @@
         <v>32</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added and updated stuff
Manuel
</commit_message>
<xml_diff>
--- a/Zeitplan/Aktueller Zeitplan.xlsx
+++ b/Zeitplan/Aktueller Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Info\Projects\UniprojektGitHub\Zeitplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC608FB-9FE2-480D-A309-4E7125A45196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623BAF30-597D-4CEB-AF56-AC8F4E33C054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{3BCD9E55-44D3-4FC7-AA79-02F85DDF559B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t xml:space="preserve">Tag </t>
   </si>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184A74EC-D31E-49F0-BF6D-A9373D7AB90E}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -779,6 +779,9 @@
       <c r="L5" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="M5" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -817,6 +820,9 @@
       <c r="L6" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="M6" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -855,6 +861,9 @@
       <c r="L7" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="M7" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -890,6 +899,12 @@
       <c r="K8" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="L8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -926,6 +941,9 @@
         <v>32</v>
       </c>
       <c r="L9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated LaTeXHelper and documentation
Manuel
</commit_message>
<xml_diff>
--- a/Zeitplan/Aktueller Zeitplan.xlsx
+++ b/Zeitplan/Aktueller Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Info\Projects\UniprojektGitHub\Zeitplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623BAF30-597D-4CEB-AF56-AC8F4E33C054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8F9275-D721-4458-9A09-2464DF685DD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{3BCD9E55-44D3-4FC7-AA79-02F85DDF559B}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>